<commit_message>
correcao > > rascunho
</commit_message>
<xml_diff>
--- a/public/model-export/FOLHA DE MEDICAO.xlsx
+++ b/public/model-export/FOLHA DE MEDICAO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabriciogama\Downloads\Programas\desope_tecnica-main\public\model-export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabriciogama\Downloads\desope_tecnica\public\model-export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3932668-5290-4B18-9BED-F8E14366AFA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AF2785-ADAF-4B24-A57B-45D6D279B05E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>Descrição do Serviço</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Contrato:</t>
+  </si>
+  <si>
+    <t>Outros:</t>
   </si>
 </sst>
 </file>
@@ -759,7 +762,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -887,7 +890,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1093,6 +1095,21 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1101,31 +1118,115 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1137,6 +1238,21 @@
     <xf numFmtId="165" fontId="23" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1146,125 +1262,20 @@
     <xf numFmtId="0" fontId="23" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -3430,7 +3441,7 @@
   <dimension ref="A1:O222"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="77" zoomScaleNormal="77" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:M3"/>
+      <selection activeCell="K11" sqref="K11:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3493,882 +3504,884 @@
     </row>
     <row r="3" spans="1:15" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="25"/>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
-      <c r="L3" s="169"/>
-      <c r="M3" s="169"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
       <c r="N3" s="25"/>
       <c r="O3" s="26"/>
     </row>
-    <row r="4" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="43"/>
       <c r="B4" s="44"/>
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
       <c r="J4" s="47"/>
-      <c r="K4" s="58"/>
+      <c r="K4" s="57"/>
       <c r="O4" s="26"/>
     </row>
-    <row r="5" spans="1:15" s="50" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="49" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="43"/>
       <c r="B5" s="44"/>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
       <c r="I5" s="43"/>
       <c r="J5" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="170"/>
+      <c r="K5" s="122"/>
       <c r="L5" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="179"/>
-      <c r="N5" s="179"/>
-      <c r="O5" s="74"/>
-    </row>
-    <row r="6" spans="1:15" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
+      <c r="O5" s="179"/>
+    </row>
+    <row r="6" spans="1:15" s="49" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="43"/>
       <c r="B6" s="44"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
       <c r="H6" s="46"/>
       <c r="I6" s="46"/>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="171"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="49"/>
-    </row>
-    <row r="7" spans="1:15" s="53" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="54" t="s">
+      <c r="K6" s="123"/>
+      <c r="L6" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="180"/>
+      <c r="N6" s="180"/>
+      <c r="O6" s="181"/>
+    </row>
+    <row r="7" spans="1:15" s="52" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="173"/>
-      <c r="D7" s="173"/>
-      <c r="E7" s="173"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="53" t="s">
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="55"/>
+      <c r="H7" s="54"/>
       <c r="I7" s="48"/>
-      <c r="J7" s="56" t="s">
+      <c r="J7" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="171"/>
-      <c r="L7" s="54"/>
-      <c r="O7" s="57"/>
-    </row>
-    <row r="8" spans="1:15" s="53" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B8" s="54" t="s">
+      <c r="K7" s="123"/>
+      <c r="L7" s="53"/>
+      <c r="O7" s="56"/>
+    </row>
+    <row r="8" spans="1:15" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B8" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="174"/>
-      <c r="D8" s="174"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="175"/>
-      <c r="G8" s="58" t="s">
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="56" t="s">
+      <c r="H8" s="58"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="172"/>
-      <c r="L8" s="61"/>
-      <c r="O8" s="57"/>
-    </row>
-    <row r="9" spans="1:15" s="53" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B9" s="54" t="s">
+      <c r="K8" s="124"/>
+      <c r="L8" s="60"/>
+      <c r="O8" s="56"/>
+    </row>
+    <row r="9" spans="1:15" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B9" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="176"/>
-      <c r="D9" s="177"/>
-      <c r="E9" s="177"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="58" t="s">
+      <c r="C9" s="159"/>
+      <c r="D9" s="160"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="62"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="61"/>
       <c r="J9" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="143"/>
-      <c r="L9" s="143"/>
-      <c r="O9" s="57"/>
-    </row>
-    <row r="10" spans="1:15" s="53" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B10" s="54" t="s">
+      <c r="K9" s="148"/>
+      <c r="L9" s="148"/>
+      <c r="O9" s="56"/>
+    </row>
+    <row r="10" spans="1:15" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B10" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="173"/>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="58" t="s">
+      <c r="C10" s="147"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="147"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="61"/>
       <c r="J10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="143"/>
-      <c r="L10" s="143"/>
-      <c r="O10" s="57"/>
-    </row>
-    <row r="11" spans="1:15" s="53" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B11" s="54" t="s">
+      <c r="K10" s="148"/>
+      <c r="L10" s="148"/>
+      <c r="O10" s="56"/>
+    </row>
+    <row r="11" spans="1:15" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B11" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="178"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="178"/>
-      <c r="G11" s="54" t="s">
+      <c r="C11" s="169"/>
+      <c r="D11" s="169"/>
+      <c r="E11" s="169"/>
+      <c r="F11" s="169"/>
+      <c r="G11" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="143"/>
-      <c r="I11" s="143"/>
+      <c r="H11" s="148"/>
+      <c r="I11" s="148"/>
       <c r="J11" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="143"/>
-      <c r="L11" s="143"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="65"/>
-    </row>
-    <row r="12" spans="1:15" s="53" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B12" s="54" t="s">
+      <c r="K11" s="148"/>
+      <c r="L11" s="148"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="64"/>
+    </row>
+    <row r="12" spans="1:15" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B12" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="173"/>
-      <c r="D12" s="173"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
       <c r="G12" s="44"/>
       <c r="H12" s="44"/>
       <c r="I12" s="44"/>
-      <c r="J12" s="66" t="s">
+      <c r="J12" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="143"/>
-      <c r="L12" s="143"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="65"/>
-    </row>
-    <row r="13" spans="1:15" s="53" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B13" s="54" t="s">
+      <c r="K12" s="148"/>
+      <c r="L12" s="148"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="64"/>
+    </row>
+    <row r="13" spans="1:15" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B13" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="177"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
+      <c r="C13" s="160"/>
+      <c r="D13" s="160"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
       <c r="I13" s="44"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="70"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="69"/>
       <c r="N13" s="44"/>
-      <c r="O13" s="57"/>
-    </row>
-    <row r="14" spans="1:15" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="O13" s="56"/>
+    </row>
+    <row r="14" spans="1:15" s="49" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="43"/>
-      <c r="B14" s="71"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="74"/>
-    </row>
-    <row r="15" spans="1:15" s="77" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="75"/>
-      <c r="B15" s="137" t="s">
+      <c r="B14" s="70"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="73"/>
+    </row>
+    <row r="15" spans="1:15" s="76" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="74"/>
+      <c r="B15" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="139"/>
-      <c r="F15" s="121" t="s">
+      <c r="C15" s="175"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="176"/>
+      <c r="F15" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="76" t="s">
+      <c r="G15" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="76" t="s">
+      <c r="H15" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="76" t="s">
+      <c r="I15" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="76" t="s">
+      <c r="J15" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="K15" s="76" t="s">
+      <c r="K15" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="76" t="s">
+      <c r="L15" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="133" t="s">
+      <c r="M15" s="173" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="133"/>
-      <c r="O15" s="133"/>
-    </row>
-    <row r="16" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="78">
+      <c r="N15" s="173"/>
+      <c r="O15" s="173"/>
+    </row>
+    <row r="16" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="77">
         <v>1</v>
       </c>
-      <c r="B16" s="140"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="134"/>
-      <c r="N16" s="135"/>
-      <c r="O16" s="136"/>
-    </row>
-    <row r="17" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="78">
+      <c r="B16" s="170"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="83"/>
+      <c r="M16" s="166"/>
+      <c r="N16" s="167"/>
+      <c r="O16" s="168"/>
+    </row>
+    <row r="17" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A17" s="77">
         <v>2</v>
       </c>
-      <c r="B17" s="140"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="141"/>
-      <c r="E17" s="142"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="84"/>
-      <c r="M17" s="134"/>
-      <c r="N17" s="135"/>
-      <c r="O17" s="136"/>
-    </row>
-    <row r="18" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="78">
+      <c r="B17" s="170"/>
+      <c r="C17" s="171"/>
+      <c r="D17" s="171"/>
+      <c r="E17" s="172"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="166"/>
+      <c r="N17" s="167"/>
+      <c r="O17" s="168"/>
+    </row>
+    <row r="18" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="77">
         <v>3</v>
       </c>
-      <c r="B18" s="140"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="142"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="84"/>
-      <c r="M18" s="134"/>
-      <c r="N18" s="135"/>
-      <c r="O18" s="136"/>
-    </row>
-    <row r="19" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="78">
+      <c r="B18" s="170"/>
+      <c r="C18" s="171"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="166"/>
+      <c r="N18" s="167"/>
+      <c r="O18" s="168"/>
+    </row>
+    <row r="19" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="77">
         <v>4</v>
       </c>
-      <c r="B19" s="140"/>
-      <c r="C19" s="141"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="122"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="134"/>
-      <c r="N19" s="135"/>
-      <c r="O19" s="136"/>
-    </row>
-    <row r="20" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A20" s="78">
+      <c r="B19" s="170"/>
+      <c r="C19" s="171"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
+      <c r="F19" s="121"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="166"/>
+      <c r="N19" s="167"/>
+      <c r="O19" s="168"/>
+    </row>
+    <row r="20" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" s="77">
         <v>5</v>
       </c>
-      <c r="B20" s="140"/>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="142"/>
-      <c r="F20" s="122"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="84"/>
-      <c r="M20" s="134"/>
-      <c r="N20" s="135"/>
-      <c r="O20" s="136"/>
-    </row>
-    <row r="21" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A21" s="78">
+      <c r="B20" s="170"/>
+      <c r="C20" s="171"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="121"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="166"/>
+      <c r="N20" s="167"/>
+      <c r="O20" s="168"/>
+    </row>
+    <row r="21" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A21" s="77">
         <v>6</v>
       </c>
-      <c r="B21" s="140"/>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
-      <c r="E21" s="142"/>
-      <c r="F21" s="122"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="84"/>
-      <c r="M21" s="134"/>
-      <c r="N21" s="135"/>
-      <c r="O21" s="136"/>
-    </row>
-    <row r="22" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="78">
+      <c r="B21" s="170"/>
+      <c r="C21" s="171"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="172"/>
+      <c r="F21" s="121"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="166"/>
+      <c r="N21" s="167"/>
+      <c r="O21" s="168"/>
+    </row>
+    <row r="22" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A22" s="77">
         <v>7</v>
       </c>
-      <c r="B22" s="140"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="142"/>
-      <c r="F22" s="122"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="134"/>
-      <c r="N22" s="135"/>
-      <c r="O22" s="136"/>
-    </row>
-    <row r="23" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="78">
+      <c r="B22" s="170"/>
+      <c r="C22" s="171"/>
+      <c r="D22" s="171"/>
+      <c r="E22" s="172"/>
+      <c r="F22" s="121"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="166"/>
+      <c r="N22" s="167"/>
+      <c r="O22" s="168"/>
+    </row>
+    <row r="23" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A23" s="77">
         <v>8</v>
       </c>
-      <c r="B23" s="140"/>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="142"/>
-      <c r="F23" s="122"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="134"/>
-      <c r="N23" s="135"/>
-      <c r="O23" s="136"/>
-    </row>
-    <row r="24" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="78">
+      <c r="B23" s="170"/>
+      <c r="C23" s="171"/>
+      <c r="D23" s="171"/>
+      <c r="E23" s="172"/>
+      <c r="F23" s="121"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="166"/>
+      <c r="N23" s="167"/>
+      <c r="O23" s="168"/>
+    </row>
+    <row r="24" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A24" s="77">
         <v>9</v>
       </c>
-      <c r="B24" s="140"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
-      <c r="E24" s="142"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="84"/>
-      <c r="M24" s="134"/>
-      <c r="N24" s="135"/>
-      <c r="O24" s="136"/>
-    </row>
-    <row r="25" spans="1:15" s="85" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="78">
+      <c r="B24" s="170"/>
+      <c r="C24" s="171"/>
+      <c r="D24" s="171"/>
+      <c r="E24" s="172"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="166"/>
+      <c r="N24" s="167"/>
+      <c r="O24" s="168"/>
+    </row>
+    <row r="25" spans="1:15" s="84" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A25" s="77">
         <v>10</v>
       </c>
-      <c r="B25" s="140"/>
-      <c r="C25" s="141"/>
-      <c r="D25" s="141"/>
-      <c r="E25" s="142"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="84"/>
-      <c r="M25" s="134"/>
-      <c r="N25" s="135"/>
-      <c r="O25" s="136"/>
+      <c r="B25" s="170"/>
+      <c r="C25" s="171"/>
+      <c r="D25" s="171"/>
+      <c r="E25" s="172"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="81"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="166"/>
+      <c r="N25" s="167"/>
+      <c r="O25" s="168"/>
     </row>
     <row r="26" spans="1:15" s="45" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="48"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="90" t="s">
+      <c r="B26" s="85"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="88"/>
+      <c r="K26" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="91"/>
-      <c r="M26" s="92"/>
-      <c r="N26" s="93"/>
-      <c r="O26" s="94"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="91"/>
+      <c r="N26" s="92"/>
+      <c r="O26" s="93"/>
     </row>
     <row r="27" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="48"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="96"/>
-      <c r="M27" s="92"/>
-      <c r="N27" s="93"/>
-      <c r="O27" s="94"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="95"/>
+      <c r="M27" s="91"/>
+      <c r="N27" s="92"/>
+      <c r="O27" s="93"/>
     </row>
     <row r="28" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="48"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="120" t="s">
+      <c r="B28" s="85"/>
+      <c r="C28" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="92"/>
-      <c r="N28" s="93"/>
-      <c r="O28" s="94"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="88"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="95"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="92"/>
+      <c r="O28" s="93"/>
     </row>
     <row r="29" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="48"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="119"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="88"/>
-      <c r="I29" s="88"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="95"/>
-      <c r="L29" s="96"/>
-      <c r="M29" s="92"/>
-      <c r="N29" s="93"/>
-      <c r="O29" s="94"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="95"/>
+      <c r="M29" s="91"/>
+      <c r="N29" s="92"/>
+      <c r="O29" s="93"/>
     </row>
     <row r="30" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="48"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="88"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="96"/>
-      <c r="M30" s="92"/>
-      <c r="N30" s="93"/>
-      <c r="O30" s="94"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="95"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="92"/>
+      <c r="O30" s="93"/>
     </row>
     <row r="31" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="48"/>
-      <c r="B31" s="97"/>
-      <c r="C31" s="111"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="94"/>
-    </row>
-    <row r="32" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="98"/>
-      <c r="B32" s="97" t="s">
+      <c r="B31" s="96"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="93"/>
+    </row>
+    <row r="32" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="97"/>
+      <c r="B32" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="111"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="128" t="s">
+      <c r="C32" s="110"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="K32" s="129"/>
-      <c r="L32" s="129"/>
-      <c r="M32" s="129"/>
-      <c r="N32" s="129"/>
-      <c r="O32" s="130"/>
-    </row>
-    <row r="33" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="51"/>
-      <c r="B33" s="97"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="100" t="s">
+      <c r="K32" s="162"/>
+      <c r="L32" s="162"/>
+      <c r="M32" s="162"/>
+      <c r="N32" s="162"/>
+      <c r="O32" s="163"/>
+    </row>
+    <row r="33" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="50"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="110"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="K33" s="101" t="s">
+      <c r="K33" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="L33" s="131" t="s">
+      <c r="L33" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="132"/>
-      <c r="N33" s="131"/>
-      <c r="O33" s="132"/>
-    </row>
-    <row r="34" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="98"/>
-      <c r="B34" s="97" t="s">
+      <c r="M33" s="150"/>
+      <c r="N33" s="149"/>
+      <c r="O33" s="150"/>
+    </row>
+    <row r="34" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="97"/>
+      <c r="B34" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="111"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="99"/>
-      <c r="J34" s="102" t="s">
+      <c r="C34" s="110"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="K34" s="102"/>
-      <c r="L34" s="125"/>
-      <c r="M34" s="126"/>
-      <c r="N34" s="125"/>
-      <c r="O34" s="126"/>
-    </row>
-    <row r="35" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="51"/>
-      <c r="B35" s="97"/>
-      <c r="C35" s="112"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="102" t="s">
+      <c r="K34" s="101"/>
+      <c r="L34" s="164"/>
+      <c r="M34" s="165"/>
+      <c r="N34" s="164"/>
+      <c r="O34" s="165"/>
+    </row>
+    <row r="35" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="50"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="102"/>
-      <c r="L35" s="125"/>
-      <c r="M35" s="126"/>
-      <c r="N35" s="125"/>
-      <c r="O35" s="126"/>
-    </row>
-    <row r="36" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="51"/>
-      <c r="B36" s="103"/>
-      <c r="C36" s="113"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="G36" s="104"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="102" t="s">
+      <c r="K35" s="101"/>
+      <c r="L35" s="164"/>
+      <c r="M35" s="165"/>
+      <c r="N35" s="164"/>
+      <c r="O35" s="165"/>
+    </row>
+    <row r="36" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="50"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="112"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="G36" s="103"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="102"/>
-      <c r="L36" s="125"/>
-      <c r="M36" s="126"/>
-      <c r="N36" s="125"/>
-      <c r="O36" s="126"/>
-    </row>
-    <row r="37" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="99"/>
-      <c r="B37" s="103"/>
-      <c r="C37" s="113"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="G37" s="104"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="102" t="s">
+      <c r="K36" s="101"/>
+      <c r="L36" s="164"/>
+      <c r="M36" s="165"/>
+      <c r="N36" s="164"/>
+      <c r="O36" s="165"/>
+    </row>
+    <row r="37" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="98"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="G37" s="103"/>
+      <c r="I37" s="98"/>
+      <c r="J37" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="K37" s="102"/>
-      <c r="L37" s="125"/>
-      <c r="M37" s="126"/>
-      <c r="N37" s="125"/>
-      <c r="O37" s="126"/>
-    </row>
-    <row r="38" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="104"/>
-      <c r="B38" s="103"/>
-      <c r="C38" s="114"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="G38" s="104"/>
-      <c r="I38" s="99"/>
-      <c r="J38" s="105" t="s">
+      <c r="K37" s="101"/>
+      <c r="L37" s="164"/>
+      <c r="M37" s="165"/>
+      <c r="N37" s="164"/>
+      <c r="O37" s="165"/>
+    </row>
+    <row r="38" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="103"/>
+      <c r="B38" s="102"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="G38" s="103"/>
+      <c r="I38" s="98"/>
+      <c r="J38" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="K38" s="105"/>
-      <c r="L38" s="127"/>
-      <c r="M38" s="126"/>
-      <c r="N38" s="125"/>
-      <c r="O38" s="126"/>
-    </row>
-    <row r="39" spans="1:15" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="104"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="113"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="G39" s="104"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="106"/>
+      <c r="K38" s="104"/>
+      <c r="L38" s="177"/>
+      <c r="M38" s="165"/>
+      <c r="N38" s="164"/>
+      <c r="O38" s="165"/>
+    </row>
+    <row r="39" spans="1:15" s="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="103"/>
+      <c r="B39" s="102"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="G39" s="103"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="105"/>
       <c r="M39" s="48"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="107"/>
-    </row>
-    <row r="40" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="104"/>
-      <c r="B40" s="103"/>
-      <c r="C40" s="115"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="104"/>
-      <c r="I40" s="104"/>
-      <c r="J40" s="128" t="s">
+      <c r="N39" s="50"/>
+      <c r="O39" s="106"/>
+    </row>
+    <row r="40" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="103"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="114"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="K40" s="129"/>
-      <c r="L40" s="129"/>
-      <c r="M40" s="129"/>
-      <c r="N40" s="129"/>
-      <c r="O40" s="130"/>
-    </row>
-    <row r="41" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="104"/>
-      <c r="B41" s="103"/>
-      <c r="C41" s="116"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="104"/>
-      <c r="I41" s="104"/>
-      <c r="J41" s="100" t="s">
+      <c r="K40" s="162"/>
+      <c r="L40" s="162"/>
+      <c r="M40" s="162"/>
+      <c r="N40" s="162"/>
+      <c r="O40" s="163"/>
+    </row>
+    <row r="41" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="103"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="103"/>
+      <c r="I41" s="103"/>
+      <c r="J41" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="K41" s="101" t="s">
+      <c r="K41" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="L41" s="131" t="s">
+      <c r="L41" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="M41" s="132"/>
-      <c r="N41" s="131"/>
-      <c r="O41" s="132"/>
-    </row>
-    <row r="42" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="104"/>
-      <c r="B42" s="103"/>
-      <c r="C42" s="114"/>
-      <c r="D42" s="108"/>
-      <c r="E42" s="108"/>
-      <c r="F42" s="108"/>
-      <c r="G42" s="104"/>
-      <c r="I42" s="104"/>
-      <c r="J42" s="102" t="s">
+      <c r="M41" s="150"/>
+      <c r="N41" s="149"/>
+      <c r="O41" s="150"/>
+    </row>
+    <row r="42" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="103"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="107"/>
+      <c r="E42" s="107"/>
+      <c r="F42" s="107"/>
+      <c r="G42" s="103"/>
+      <c r="I42" s="103"/>
+      <c r="J42" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="K42" s="102"/>
-      <c r="L42" s="125"/>
-      <c r="M42" s="126"/>
-      <c r="N42" s="125"/>
-      <c r="O42" s="126"/>
-    </row>
-    <row r="43" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="104"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="116"/>
-      <c r="G43" s="104"/>
-      <c r="I43" s="104"/>
-      <c r="J43" s="102" t="s">
+      <c r="K42" s="101"/>
+      <c r="L42" s="164"/>
+      <c r="M42" s="165"/>
+      <c r="N42" s="164"/>
+      <c r="O42" s="165"/>
+    </row>
+    <row r="43" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="103"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="115"/>
+      <c r="G43" s="103"/>
+      <c r="I43" s="103"/>
+      <c r="J43" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="K43" s="102"/>
-      <c r="L43" s="125"/>
-      <c r="M43" s="126"/>
-      <c r="N43" s="125"/>
-      <c r="O43" s="126"/>
-    </row>
-    <row r="44" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="104"/>
-      <c r="B44" s="103"/>
-      <c r="C44" s="116"/>
-      <c r="D44" s="104"/>
-      <c r="E44" s="104"/>
-      <c r="F44" s="104"/>
-      <c r="G44" s="104"/>
-      <c r="I44" s="104"/>
-      <c r="J44" s="102" t="s">
+      <c r="K43" s="101"/>
+      <c r="L43" s="164"/>
+      <c r="M43" s="165"/>
+      <c r="N43" s="164"/>
+      <c r="O43" s="165"/>
+    </row>
+    <row r="44" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="103"/>
+      <c r="B44" s="102"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="103"/>
+      <c r="E44" s="103"/>
+      <c r="F44" s="103"/>
+      <c r="G44" s="103"/>
+      <c r="I44" s="103"/>
+      <c r="J44" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="K44" s="102"/>
-      <c r="L44" s="165"/>
-      <c r="M44" s="165"/>
-      <c r="N44" s="165"/>
-      <c r="O44" s="165"/>
-    </row>
-    <row r="45" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="104"/>
-      <c r="B45" s="103"/>
-      <c r="C45" s="117"/>
-      <c r="D45" s="104"/>
-      <c r="E45" s="104"/>
-      <c r="F45" s="104"/>
-      <c r="G45" s="104"/>
-      <c r="I45" s="104"/>
-      <c r="J45" s="102" t="s">
+      <c r="K44" s="101"/>
+      <c r="L44" s="140"/>
+      <c r="M44" s="140"/>
+      <c r="N44" s="140"/>
+      <c r="O44" s="140"/>
+    </row>
+    <row r="45" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="103"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="103"/>
+      <c r="E45" s="103"/>
+      <c r="F45" s="103"/>
+      <c r="G45" s="103"/>
+      <c r="I45" s="103"/>
+      <c r="J45" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="K45" s="102"/>
-      <c r="L45" s="165"/>
-      <c r="M45" s="165"/>
-      <c r="N45" s="165"/>
-      <c r="O45" s="165"/>
-    </row>
-    <row r="46" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="104"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="116"/>
-      <c r="D46" s="104"/>
-      <c r="E46" s="104"/>
-      <c r="F46" s="104"/>
-      <c r="G46" s="104"/>
-      <c r="I46" s="104"/>
-      <c r="J46" s="105" t="s">
+      <c r="K45" s="101"/>
+      <c r="L45" s="140"/>
+      <c r="M45" s="140"/>
+      <c r="N45" s="140"/>
+      <c r="O45" s="140"/>
+    </row>
+    <row r="46" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="103"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="115"/>
+      <c r="D46" s="103"/>
+      <c r="E46" s="103"/>
+      <c r="F46" s="103"/>
+      <c r="G46" s="103"/>
+      <c r="I46" s="103"/>
+      <c r="J46" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="K46" s="105"/>
-      <c r="L46" s="165"/>
-      <c r="M46" s="165"/>
-      <c r="N46" s="165"/>
-      <c r="O46" s="165"/>
-    </row>
-    <row r="47" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="104"/>
-      <c r="B47" s="103"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="104"/>
-      <c r="E47" s="104"/>
-      <c r="F47" s="104"/>
-      <c r="G47" s="104"/>
-      <c r="I47" s="104"/>
-      <c r="J47" s="104"/>
-      <c r="K47" s="104"/>
-      <c r="L47" s="104"/>
-      <c r="M47" s="104"/>
-      <c r="N47" s="104"/>
-      <c r="O47" s="109"/>
-    </row>
-    <row r="48" spans="1:15" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="104"/>
-      <c r="B48" s="103"/>
-      <c r="C48" s="113"/>
-      <c r="D48" s="104"/>
-      <c r="E48" s="104"/>
-      <c r="F48" s="104"/>
-      <c r="G48" s="104"/>
-      <c r="I48" s="104"/>
-      <c r="J48" s="104"/>
-      <c r="K48" s="104"/>
-      <c r="L48" s="104"/>
-      <c r="M48" s="104"/>
-      <c r="N48" s="104"/>
-      <c r="O48" s="109"/>
-    </row>
-    <row r="49" spans="1:15" s="77" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A49" s="104"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="113"/>
-      <c r="D49" s="104"/>
-      <c r="E49" s="104"/>
-      <c r="F49" s="104"/>
-      <c r="G49" s="104"/>
-      <c r="I49" s="104"/>
-      <c r="J49" s="104"/>
-      <c r="K49" s="104"/>
-      <c r="L49" s="104"/>
-      <c r="M49" s="104"/>
-      <c r="N49" s="104"/>
-      <c r="O49" s="109"/>
+      <c r="K46" s="104"/>
+      <c r="L46" s="140"/>
+      <c r="M46" s="140"/>
+      <c r="N46" s="140"/>
+      <c r="O46" s="140"/>
+    </row>
+    <row r="47" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="103"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="115"/>
+      <c r="D47" s="103"/>
+      <c r="E47" s="103"/>
+      <c r="F47" s="103"/>
+      <c r="G47" s="103"/>
+      <c r="I47" s="103"/>
+      <c r="J47" s="103"/>
+      <c r="K47" s="103"/>
+      <c r="L47" s="103"/>
+      <c r="M47" s="103"/>
+      <c r="N47" s="103"/>
+      <c r="O47" s="108"/>
+    </row>
+    <row r="48" spans="1:15" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="103"/>
+      <c r="B48" s="102"/>
+      <c r="C48" s="112"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="103"/>
+      <c r="F48" s="103"/>
+      <c r="G48" s="103"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="103"/>
+      <c r="K48" s="103"/>
+      <c r="L48" s="103"/>
+      <c r="M48" s="103"/>
+      <c r="N48" s="103"/>
+      <c r="O48" s="108"/>
+    </row>
+    <row r="49" spans="1:15" s="76" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A49" s="103"/>
+      <c r="B49" s="102"/>
+      <c r="C49" s="112"/>
+      <c r="D49" s="103"/>
+      <c r="E49" s="103"/>
+      <c r="F49" s="103"/>
+      <c r="G49" s="103"/>
+      <c r="I49" s="103"/>
+      <c r="J49" s="103"/>
+      <c r="K49" s="103"/>
+      <c r="L49" s="103"/>
+      <c r="M49" s="103"/>
+      <c r="N49" s="103"/>
+      <c r="O49" s="108"/>
     </row>
     <row r="50" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="118"/>
+      <c r="C50" s="117"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -4449,45 +4462,45 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="I55" s="3"/>
-      <c r="J55" s="164"/>
-      <c r="K55" s="164"/>
-      <c r="L55" s="164"/>
-      <c r="M55" s="164"/>
-      <c r="N55" s="164"/>
+      <c r="J55" s="139"/>
+      <c r="K55" s="139"/>
+      <c r="L55" s="139"/>
+      <c r="M55" s="139"/>
+      <c r="N55" s="139"/>
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="16"/>
-      <c r="C56" s="157"/>
-      <c r="D56" s="157"/>
-      <c r="E56" s="157"/>
-      <c r="F56" s="157"/>
-      <c r="G56" s="157"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="138"/>
+      <c r="E56" s="138"/>
+      <c r="F56" s="138"/>
+      <c r="G56" s="138"/>
       <c r="I56" s="5"/>
-      <c r="J56" s="164"/>
-      <c r="K56" s="164"/>
-      <c r="L56" s="164"/>
-      <c r="M56" s="164"/>
-      <c r="N56" s="164"/>
+      <c r="J56" s="139"/>
+      <c r="K56" s="139"/>
+      <c r="L56" s="139"/>
+      <c r="M56" s="139"/>
+      <c r="N56" s="139"/>
       <c r="O56" s="9"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="16"/>
-      <c r="C57" s="161" t="s">
+      <c r="C57" s="158" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="161"/>
-      <c r="E57" s="161"/>
-      <c r="F57" s="161"/>
-      <c r="G57" s="161"/>
+      <c r="D57" s="158"/>
+      <c r="E57" s="158"/>
+      <c r="F57" s="158"/>
+      <c r="G57" s="158"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="157"/>
-      <c r="K57" s="157"/>
-      <c r="L57" s="157"/>
-      <c r="M57" s="157"/>
-      <c r="N57" s="157"/>
+      <c r="J57" s="138"/>
+      <c r="K57" s="138"/>
+      <c r="L57" s="138"/>
+      <c r="M57" s="138"/>
+      <c r="N57" s="138"/>
       <c r="O57" s="9"/>
     </row>
     <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.3">
@@ -4495,19 +4508,19 @@
       <c r="B58" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="162" t="s">
+      <c r="C58" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="D58" s="162"/>
-      <c r="E58" s="162"/>
-      <c r="F58" s="162"/>
-      <c r="G58" s="162"/>
+      <c r="D58" s="136"/>
+      <c r="E58" s="136"/>
+      <c r="F58" s="136"/>
+      <c r="G58" s="136"/>
       <c r="I58" s="3"/>
       <c r="J58" s="5"/>
-      <c r="K58" s="163" t="s">
+      <c r="K58" s="137" t="s">
         <v>50</v>
       </c>
-      <c r="L58" s="163"/>
+      <c r="L58" s="137"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="9"/>
@@ -4517,17 +4530,17 @@
       <c r="B59" s="16"/>
       <c r="C59" s="3"/>
       <c r="D59" s="14"/>
-      <c r="E59" s="153" t="s">
+      <c r="E59" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="F59" s="153"/>
+      <c r="F59" s="151"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
-      <c r="K59" s="154" t="s">
+      <c r="K59" s="152" t="s">
         <v>48</v>
       </c>
-      <c r="L59" s="154"/>
+      <c r="L59" s="152"/>
       <c r="M59" s="10"/>
       <c r="N59" s="10"/>
       <c r="O59" s="9"/>
@@ -4543,10 +4556,10 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
-      <c r="K60" s="157" t="s">
+      <c r="K60" s="138" t="s">
         <v>49</v>
       </c>
-      <c r="L60" s="157"/>
+      <c r="L60" s="138"/>
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
       <c r="O60" s="11"/>
@@ -4584,22 +4597,22 @@
       <c r="O62" s="3"/>
     </row>
     <row r="63" spans="1:15" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="155" t="s">
+      <c r="A63" s="153" t="s">
         <v>34</v>
       </c>
-      <c r="B63" s="155"/>
-      <c r="C63" s="155"/>
-      <c r="D63" s="155"/>
-      <c r="E63" s="155"/>
-      <c r="F63" s="155"/>
-      <c r="G63" s="155"/>
-      <c r="H63" s="155"/>
-      <c r="I63" s="155"/>
-      <c r="J63" s="155"/>
-      <c r="K63" s="155"/>
-      <c r="L63" s="155"/>
-      <c r="M63" s="155"/>
-      <c r="N63" s="155"/>
+      <c r="B63" s="153"/>
+      <c r="C63" s="153"/>
+      <c r="D63" s="153"/>
+      <c r="E63" s="153"/>
+      <c r="F63" s="153"/>
+      <c r="G63" s="153"/>
+      <c r="H63" s="153"/>
+      <c r="I63" s="153"/>
+      <c r="J63" s="153"/>
+      <c r="K63" s="153"/>
+      <c r="L63" s="153"/>
+      <c r="M63" s="153"/>
+      <c r="N63" s="153"/>
       <c r="O63" s="3"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -4619,12 +4632,12 @@
       <c r="O64" s="3"/>
     </row>
     <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.3">
-      <c r="A65" s="156" t="s">
+      <c r="A65" s="154" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="156"/>
-      <c r="C65" s="157"/>
-      <c r="D65" s="157"/>
+      <c r="B65" s="154"/>
+      <c r="C65" s="138"/>
+      <c r="D65" s="138"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -4653,33 +4666,33 @@
       <c r="O66" s="3"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A67" s="158" t="s">
+      <c r="A67" s="155" t="s">
         <v>36</v>
       </c>
-      <c r="B67" s="159"/>
-      <c r="C67" s="159"/>
-      <c r="D67" s="159"/>
-      <c r="E67" s="159"/>
-      <c r="F67" s="159"/>
-      <c r="G67" s="160"/>
+      <c r="B67" s="156"/>
+      <c r="C67" s="156"/>
+      <c r="D67" s="156"/>
+      <c r="E67" s="156"/>
+      <c r="F67" s="156"/>
+      <c r="G67" s="157"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
-      <c r="J67" s="158" t="s">
+      <c r="J67" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="K67" s="159"/>
-      <c r="L67" s="159"/>
-      <c r="M67" s="159"/>
-      <c r="N67" s="159"/>
-      <c r="O67" s="160"/>
+      <c r="K67" s="156"/>
+      <c r="L67" s="156"/>
+      <c r="M67" s="156"/>
+      <c r="N67" s="156"/>
+      <c r="O67" s="157"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="147" t="s">
+      <c r="A68" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="148"/>
-      <c r="C68" s="148"/>
-      <c r="D68" s="149"/>
+      <c r="B68" s="142"/>
+      <c r="C68" s="142"/>
+      <c r="D68" s="143"/>
       <c r="E68" s="28" t="s">
         <v>39</v>
       </c>
@@ -4691,509 +4704,509 @@
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
-      <c r="J68" s="150" t="s">
+      <c r="J68" s="144" t="s">
         <v>38</v>
       </c>
-      <c r="K68" s="151"/>
+      <c r="K68" s="145"/>
       <c r="L68" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="M68" s="147" t="s">
+      <c r="M68" s="141" t="s">
         <v>40</v>
       </c>
-      <c r="N68" s="151"/>
+      <c r="N68" s="145"/>
       <c r="O68" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A69" s="144"/>
-      <c r="B69" s="144"/>
-      <c r="C69" s="144"/>
-      <c r="D69" s="144"/>
+      <c r="A69" s="133"/>
+      <c r="B69" s="133"/>
+      <c r="C69" s="133"/>
+      <c r="D69" s="133"/>
       <c r="E69" s="42"/>
       <c r="F69" s="38"/>
       <c r="G69" s="30"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
-      <c r="J69" s="145"/>
-      <c r="K69" s="146"/>
+      <c r="J69" s="134"/>
+      <c r="K69" s="135"/>
       <c r="L69" s="42"/>
-      <c r="M69" s="123"/>
-      <c r="N69" s="124"/>
+      <c r="M69" s="127"/>
+      <c r="N69" s="128"/>
       <c r="O69" s="41"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A70" s="144"/>
-      <c r="B70" s="144"/>
-      <c r="C70" s="144"/>
-      <c r="D70" s="144"/>
+      <c r="A70" s="133"/>
+      <c r="B70" s="133"/>
+      <c r="C70" s="133"/>
+      <c r="D70" s="133"/>
       <c r="E70" s="42"/>
       <c r="F70" s="38"/>
       <c r="G70" s="30"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
-      <c r="J70" s="145"/>
-      <c r="K70" s="146"/>
+      <c r="J70" s="134"/>
+      <c r="K70" s="135"/>
       <c r="L70" s="42"/>
-      <c r="M70" s="123"/>
-      <c r="N70" s="124"/>
+      <c r="M70" s="127"/>
+      <c r="N70" s="128"/>
       <c r="O70" s="41"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A71" s="144"/>
-      <c r="B71" s="144"/>
-      <c r="C71" s="144"/>
-      <c r="D71" s="144"/>
+      <c r="A71" s="133"/>
+      <c r="B71" s="133"/>
+      <c r="C71" s="133"/>
+      <c r="D71" s="133"/>
       <c r="E71" s="42"/>
       <c r="F71" s="38"/>
       <c r="G71" s="30"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
-      <c r="J71" s="145"/>
-      <c r="K71" s="146"/>
+      <c r="J71" s="134"/>
+      <c r="K71" s="135"/>
       <c r="L71" s="42"/>
-      <c r="M71" s="123"/>
-      <c r="N71" s="124"/>
+      <c r="M71" s="127"/>
+      <c r="N71" s="128"/>
       <c r="O71" s="41"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="144"/>
-      <c r="B72" s="144"/>
-      <c r="C72" s="144"/>
-      <c r="D72" s="144"/>
+      <c r="A72" s="133"/>
+      <c r="B72" s="133"/>
+      <c r="C72" s="133"/>
+      <c r="D72" s="133"/>
       <c r="E72" s="42"/>
       <c r="F72" s="38"/>
       <c r="G72" s="30"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
-      <c r="J72" s="145"/>
-      <c r="K72" s="146"/>
+      <c r="J72" s="134"/>
+      <c r="K72" s="135"/>
       <c r="L72" s="42"/>
-      <c r="M72" s="123"/>
-      <c r="N72" s="124"/>
+      <c r="M72" s="127"/>
+      <c r="N72" s="128"/>
       <c r="O72" s="41"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A73" s="144"/>
-      <c r="B73" s="144"/>
-      <c r="C73" s="144"/>
-      <c r="D73" s="144"/>
+      <c r="A73" s="133"/>
+      <c r="B73" s="133"/>
+      <c r="C73" s="133"/>
+      <c r="D73" s="133"/>
       <c r="E73" s="42"/>
       <c r="F73" s="38"/>
       <c r="G73" s="30"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
-      <c r="J73" s="145"/>
-      <c r="K73" s="146"/>
+      <c r="J73" s="134"/>
+      <c r="K73" s="135"/>
       <c r="L73" s="42"/>
-      <c r="M73" s="123"/>
-      <c r="N73" s="124"/>
+      <c r="M73" s="127"/>
+      <c r="N73" s="128"/>
       <c r="O73" s="41"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="144"/>
-      <c r="B74" s="144"/>
-      <c r="C74" s="144"/>
-      <c r="D74" s="144"/>
+      <c r="A74" s="133"/>
+      <c r="B74" s="133"/>
+      <c r="C74" s="133"/>
+      <c r="D74" s="133"/>
       <c r="E74" s="42"/>
       <c r="F74" s="38"/>
       <c r="G74" s="30"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
-      <c r="J74" s="145"/>
-      <c r="K74" s="146"/>
+      <c r="J74" s="134"/>
+      <c r="K74" s="135"/>
       <c r="L74" s="42"/>
-      <c r="M74" s="123"/>
-      <c r="N74" s="124"/>
+      <c r="M74" s="127"/>
+      <c r="N74" s="128"/>
       <c r="O74" s="41"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="144"/>
-      <c r="B75" s="144"/>
-      <c r="C75" s="144"/>
-      <c r="D75" s="144"/>
+      <c r="A75" s="133"/>
+      <c r="B75" s="133"/>
+      <c r="C75" s="133"/>
+      <c r="D75" s="133"/>
       <c r="E75" s="42"/>
       <c r="F75" s="38"/>
       <c r="G75" s="30"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
-      <c r="J75" s="145"/>
-      <c r="K75" s="146"/>
+      <c r="J75" s="134"/>
+      <c r="K75" s="135"/>
       <c r="L75" s="42"/>
-      <c r="M75" s="123"/>
-      <c r="N75" s="124"/>
+      <c r="M75" s="127"/>
+      <c r="N75" s="128"/>
       <c r="O75" s="41"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A76" s="144"/>
-      <c r="B76" s="144"/>
-      <c r="C76" s="144"/>
-      <c r="D76" s="144"/>
+      <c r="A76" s="133"/>
+      <c r="B76" s="133"/>
+      <c r="C76" s="133"/>
+      <c r="D76" s="133"/>
       <c r="E76" s="42"/>
       <c r="F76" s="38"/>
       <c r="G76" s="30"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
-      <c r="J76" s="145"/>
-      <c r="K76" s="146"/>
+      <c r="J76" s="134"/>
+      <c r="K76" s="135"/>
       <c r="L76" s="42"/>
-      <c r="M76" s="123"/>
-      <c r="N76" s="124"/>
+      <c r="M76" s="127"/>
+      <c r="N76" s="128"/>
       <c r="O76" s="41"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A77" s="144"/>
-      <c r="B77" s="144"/>
-      <c r="C77" s="144"/>
-      <c r="D77" s="144"/>
+      <c r="A77" s="133"/>
+      <c r="B77" s="133"/>
+      <c r="C77" s="133"/>
+      <c r="D77" s="133"/>
       <c r="E77" s="42"/>
       <c r="F77" s="38"/>
       <c r="G77" s="30"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
-      <c r="J77" s="145"/>
-      <c r="K77" s="146"/>
+      <c r="J77" s="134"/>
+      <c r="K77" s="135"/>
       <c r="L77" s="42"/>
-      <c r="M77" s="123"/>
-      <c r="N77" s="124"/>
+      <c r="M77" s="127"/>
+      <c r="N77" s="128"/>
       <c r="O77" s="41"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A78" s="144"/>
-      <c r="B78" s="144"/>
-      <c r="C78" s="144"/>
-      <c r="D78" s="144"/>
+      <c r="A78" s="133"/>
+      <c r="B78" s="133"/>
+      <c r="C78" s="133"/>
+      <c r="D78" s="133"/>
       <c r="E78" s="42"/>
       <c r="F78" s="38"/>
       <c r="G78" s="30"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
-      <c r="J78" s="145"/>
-      <c r="K78" s="146"/>
+      <c r="J78" s="134"/>
+      <c r="K78" s="135"/>
       <c r="L78" s="42"/>
-      <c r="M78" s="123"/>
-      <c r="N78" s="124"/>
+      <c r="M78" s="127"/>
+      <c r="N78" s="128"/>
       <c r="O78" s="41"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A79" s="144"/>
-      <c r="B79" s="144"/>
-      <c r="C79" s="144"/>
-      <c r="D79" s="144"/>
+      <c r="A79" s="133"/>
+      <c r="B79" s="133"/>
+      <c r="C79" s="133"/>
+      <c r="D79" s="133"/>
       <c r="E79" s="42"/>
       <c r="F79" s="38"/>
       <c r="G79" s="30"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
-      <c r="J79" s="145"/>
-      <c r="K79" s="146"/>
+      <c r="J79" s="134"/>
+      <c r="K79" s="135"/>
       <c r="L79" s="42"/>
-      <c r="M79" s="123"/>
-      <c r="N79" s="124"/>
+      <c r="M79" s="127"/>
+      <c r="N79" s="128"/>
       <c r="O79" s="41"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="144"/>
-      <c r="B80" s="144"/>
-      <c r="C80" s="144"/>
-      <c r="D80" s="144"/>
+      <c r="A80" s="133"/>
+      <c r="B80" s="133"/>
+      <c r="C80" s="133"/>
+      <c r="D80" s="133"/>
       <c r="E80" s="42"/>
       <c r="F80" s="38"/>
       <c r="G80" s="30"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
-      <c r="J80" s="145"/>
-      <c r="K80" s="146"/>
+      <c r="J80" s="134"/>
+      <c r="K80" s="135"/>
       <c r="L80" s="42"/>
-      <c r="M80" s="123"/>
-      <c r="N80" s="124"/>
+      <c r="M80" s="127"/>
+      <c r="N80" s="128"/>
       <c r="O80" s="41"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A81" s="144"/>
-      <c r="B81" s="144"/>
-      <c r="C81" s="144"/>
-      <c r="D81" s="144"/>
+      <c r="A81" s="133"/>
+      <c r="B81" s="133"/>
+      <c r="C81" s="133"/>
+      <c r="D81" s="133"/>
       <c r="E81" s="42"/>
       <c r="F81" s="38"/>
       <c r="G81" s="30"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="145"/>
-      <c r="K81" s="146"/>
+      <c r="J81" s="134"/>
+      <c r="K81" s="135"/>
       <c r="L81" s="42"/>
-      <c r="M81" s="123"/>
-      <c r="N81" s="124"/>
+      <c r="M81" s="127"/>
+      <c r="N81" s="128"/>
       <c r="O81" s="41"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A82" s="144"/>
-      <c r="B82" s="144"/>
-      <c r="C82" s="144"/>
-      <c r="D82" s="144"/>
+      <c r="A82" s="133"/>
+      <c r="B82" s="133"/>
+      <c r="C82" s="133"/>
+      <c r="D82" s="133"/>
       <c r="E82" s="42"/>
       <c r="F82" s="38"/>
       <c r="G82" s="30"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
-      <c r="J82" s="145"/>
-      <c r="K82" s="146"/>
+      <c r="J82" s="134"/>
+      <c r="K82" s="135"/>
       <c r="L82" s="42"/>
-      <c r="M82" s="123"/>
-      <c r="N82" s="124"/>
+      <c r="M82" s="127"/>
+      <c r="N82" s="128"/>
       <c r="O82" s="41"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A83" s="144"/>
-      <c r="B83" s="144"/>
-      <c r="C83" s="144"/>
-      <c r="D83" s="144"/>
+      <c r="A83" s="133"/>
+      <c r="B83" s="133"/>
+      <c r="C83" s="133"/>
+      <c r="D83" s="133"/>
       <c r="E83" s="42"/>
       <c r="F83" s="38"/>
       <c r="G83" s="30"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
-      <c r="J83" s="145"/>
-      <c r="K83" s="146"/>
+      <c r="J83" s="134"/>
+      <c r="K83" s="135"/>
       <c r="L83" s="42"/>
-      <c r="M83" s="123"/>
-      <c r="N83" s="124"/>
+      <c r="M83" s="127"/>
+      <c r="N83" s="128"/>
       <c r="O83" s="41"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A84" s="144"/>
-      <c r="B84" s="144"/>
-      <c r="C84" s="144"/>
-      <c r="D84" s="144"/>
+      <c r="A84" s="133"/>
+      <c r="B84" s="133"/>
+      <c r="C84" s="133"/>
+      <c r="D84" s="133"/>
       <c r="E84" s="42"/>
       <c r="F84" s="38"/>
       <c r="G84" s="30"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
-      <c r="J84" s="145"/>
-      <c r="K84" s="146"/>
+      <c r="J84" s="134"/>
+      <c r="K84" s="135"/>
       <c r="L84" s="42"/>
-      <c r="M84" s="123"/>
-      <c r="N84" s="124"/>
+      <c r="M84" s="127"/>
+      <c r="N84" s="128"/>
       <c r="O84" s="41"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A85" s="144"/>
-      <c r="B85" s="144"/>
-      <c r="C85" s="144"/>
-      <c r="D85" s="144"/>
+      <c r="A85" s="133"/>
+      <c r="B85" s="133"/>
+      <c r="C85" s="133"/>
+      <c r="D85" s="133"/>
       <c r="E85" s="42"/>
       <c r="F85" s="38"/>
       <c r="G85" s="30"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
-      <c r="J85" s="145"/>
-      <c r="K85" s="146"/>
+      <c r="J85" s="134"/>
+      <c r="K85" s="135"/>
       <c r="L85" s="39"/>
       <c r="M85" s="37"/>
       <c r="N85" s="40"/>
       <c r="O85" s="41"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A86" s="144"/>
-      <c r="B86" s="144"/>
-      <c r="C86" s="144"/>
-      <c r="D86" s="144"/>
+      <c r="A86" s="133"/>
+      <c r="B86" s="133"/>
+      <c r="C86" s="133"/>
+      <c r="D86" s="133"/>
       <c r="E86" s="42"/>
       <c r="F86" s="38"/>
       <c r="G86" s="30"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
-      <c r="J86" s="145"/>
-      <c r="K86" s="146"/>
+      <c r="J86" s="134"/>
+      <c r="K86" s="135"/>
       <c r="L86" s="39"/>
       <c r="M86" s="37"/>
       <c r="N86" s="40"/>
       <c r="O86" s="41"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A87" s="144"/>
-      <c r="B87" s="144"/>
-      <c r="C87" s="144"/>
-      <c r="D87" s="144"/>
+      <c r="A87" s="133"/>
+      <c r="B87" s="133"/>
+      <c r="C87" s="133"/>
+      <c r="D87" s="133"/>
       <c r="E87" s="42"/>
       <c r="F87" s="38"/>
       <c r="G87" s="30"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
-      <c r="J87" s="145"/>
-      <c r="K87" s="146"/>
+      <c r="J87" s="134"/>
+      <c r="K87" s="135"/>
       <c r="L87" s="39"/>
       <c r="M87" s="37"/>
       <c r="N87" s="40"/>
       <c r="O87" s="41"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A88" s="144"/>
-      <c r="B88" s="144"/>
-      <c r="C88" s="144"/>
-      <c r="D88" s="144"/>
+      <c r="A88" s="133"/>
+      <c r="B88" s="133"/>
+      <c r="C88" s="133"/>
+      <c r="D88" s="133"/>
       <c r="E88" s="39"/>
       <c r="F88" s="39"/>
       <c r="G88" s="30"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
-      <c r="J88" s="166"/>
-      <c r="K88" s="168"/>
+      <c r="J88" s="130"/>
+      <c r="K88" s="132"/>
       <c r="L88" s="32"/>
       <c r="M88" s="33"/>
       <c r="N88" s="34"/>
       <c r="O88" s="31"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A89" s="166"/>
-      <c r="B89" s="167"/>
-      <c r="C89" s="167"/>
-      <c r="D89" s="167"/>
+      <c r="A89" s="130"/>
+      <c r="B89" s="131"/>
+      <c r="C89" s="131"/>
+      <c r="D89" s="131"/>
       <c r="E89" s="32"/>
       <c r="F89" s="32"/>
       <c r="G89" s="32"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
-      <c r="J89" s="166"/>
-      <c r="K89" s="168"/>
+      <c r="J89" s="130"/>
+      <c r="K89" s="132"/>
       <c r="L89" s="32"/>
       <c r="M89" s="33"/>
       <c r="N89" s="34"/>
       <c r="O89" s="31"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A90" s="166"/>
-      <c r="B90" s="167"/>
-      <c r="C90" s="167"/>
-      <c r="D90" s="167"/>
+      <c r="A90" s="130"/>
+      <c r="B90" s="131"/>
+      <c r="C90" s="131"/>
+      <c r="D90" s="131"/>
       <c r="E90" s="32"/>
       <c r="F90" s="32"/>
       <c r="G90" s="32"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
-      <c r="J90" s="166"/>
-      <c r="K90" s="168"/>
+      <c r="J90" s="130"/>
+      <c r="K90" s="132"/>
       <c r="L90" s="32"/>
       <c r="M90" s="33"/>
       <c r="N90" s="34"/>
       <c r="O90" s="31"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A91" s="166"/>
-      <c r="B91" s="167"/>
-      <c r="C91" s="167"/>
-      <c r="D91" s="167"/>
+      <c r="A91" s="130"/>
+      <c r="B91" s="131"/>
+      <c r="C91" s="131"/>
+      <c r="D91" s="131"/>
       <c r="E91" s="32"/>
       <c r="F91" s="32"/>
       <c r="G91" s="32"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
-      <c r="J91" s="166"/>
-      <c r="K91" s="168"/>
+      <c r="J91" s="130"/>
+      <c r="K91" s="132"/>
       <c r="L91" s="32"/>
       <c r="M91" s="33"/>
       <c r="N91" s="34"/>
       <c r="O91" s="31"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A92" s="166"/>
-      <c r="B92" s="167"/>
-      <c r="C92" s="167"/>
-      <c r="D92" s="167"/>
+      <c r="A92" s="130"/>
+      <c r="B92" s="131"/>
+      <c r="C92" s="131"/>
+      <c r="D92" s="131"/>
       <c r="E92" s="32"/>
       <c r="F92" s="32"/>
       <c r="G92" s="32"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="166"/>
-      <c r="K92" s="168"/>
+      <c r="J92" s="130"/>
+      <c r="K92" s="132"/>
       <c r="L92" s="32"/>
       <c r="M92" s="33"/>
       <c r="N92" s="34"/>
       <c r="O92" s="31"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A93" s="166"/>
-      <c r="B93" s="167"/>
-      <c r="C93" s="167"/>
-      <c r="D93" s="167"/>
+      <c r="A93" s="130"/>
+      <c r="B93" s="131"/>
+      <c r="C93" s="131"/>
+      <c r="D93" s="131"/>
       <c r="E93" s="32"/>
       <c r="F93" s="32"/>
       <c r="G93" s="32"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-      <c r="J93" s="166"/>
-      <c r="K93" s="168"/>
+      <c r="J93" s="130"/>
+      <c r="K93" s="132"/>
       <c r="L93" s="32"/>
       <c r="M93" s="33"/>
       <c r="N93" s="34"/>
       <c r="O93" s="31"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A94" s="166"/>
-      <c r="B94" s="167"/>
-      <c r="C94" s="167"/>
-      <c r="D94" s="167"/>
+      <c r="A94" s="130"/>
+      <c r="B94" s="131"/>
+      <c r="C94" s="131"/>
+      <c r="D94" s="131"/>
       <c r="E94" s="32"/>
       <c r="F94" s="32"/>
       <c r="G94" s="32"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
-      <c r="J94" s="166"/>
-      <c r="K94" s="168"/>
+      <c r="J94" s="130"/>
+      <c r="K94" s="132"/>
       <c r="L94" s="32"/>
       <c r="M94" s="33"/>
       <c r="N94" s="34"/>
       <c r="O94" s="31"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A95" s="166"/>
-      <c r="B95" s="167"/>
-      <c r="C95" s="167"/>
-      <c r="D95" s="167"/>
+      <c r="A95" s="130"/>
+      <c r="B95" s="131"/>
+      <c r="C95" s="131"/>
+      <c r="D95" s="131"/>
       <c r="E95" s="32"/>
       <c r="F95" s="32"/>
       <c r="G95" s="32"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
-      <c r="J95" s="166"/>
-      <c r="K95" s="168"/>
+      <c r="J95" s="130"/>
+      <c r="K95" s="132"/>
       <c r="L95" s="32"/>
       <c r="M95" s="33"/>
       <c r="N95" s="34"/>
       <c r="O95" s="31"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A96" s="166"/>
-      <c r="B96" s="167"/>
-      <c r="C96" s="167"/>
-      <c r="D96" s="167"/>
+      <c r="A96" s="130"/>
+      <c r="B96" s="131"/>
+      <c r="C96" s="131"/>
+      <c r="D96" s="131"/>
       <c r="E96" s="32"/>
       <c r="F96" s="32"/>
       <c r="G96" s="32"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="166"/>
-      <c r="K96" s="168"/>
+      <c r="J96" s="130"/>
+      <c r="K96" s="132"/>
       <c r="L96" s="32"/>
       <c r="M96" s="33"/>
       <c r="N96" s="34"/>
       <c r="O96" s="31"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A97" s="166"/>
-      <c r="B97" s="167"/>
-      <c r="C97" s="167"/>
-      <c r="D97" s="167"/>
+      <c r="A97" s="130"/>
+      <c r="B97" s="131"/>
+      <c r="C97" s="131"/>
+      <c r="D97" s="131"/>
       <c r="E97" s="32"/>
       <c r="F97" s="32"/>
       <c r="G97" s="32"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
-      <c r="J97" s="166"/>
-      <c r="K97" s="168"/>
+      <c r="J97" s="130"/>
+      <c r="K97" s="132"/>
       <c r="L97" s="32"/>
       <c r="M97" s="33"/>
       <c r="N97" s="34"/>
@@ -7075,72 +7088,72 @@
       <c r="O222"/>
     </row>
   </sheetData>
-  <mergeCells count="152">
-    <mergeCell ref="M69:N69"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="J95:K95"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="J85:K85"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="M70:N70"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="J97:K97"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="J91:K91"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="J94:K94"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="J78:K78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="J73:K73"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="J74:K74"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="J55:N57"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N45:O45"/>
+  <mergeCells count="154">
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M81:N81"/>
+    <mergeCell ref="M82:N82"/>
+    <mergeCell ref="M83:N83"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="M79:N79"/>
+    <mergeCell ref="M80:N80"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="M73:N73"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M76:N76"/>
+    <mergeCell ref="M77:N77"/>
+    <mergeCell ref="M78:N78"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="J40:O40"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="A71:D71"/>
     <mergeCell ref="J71:K71"/>
     <mergeCell ref="A69:D69"/>
@@ -7165,69 +7178,71 @@
     <mergeCell ref="J67:O67"/>
     <mergeCell ref="C56:G56"/>
     <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="M81:N81"/>
-    <mergeCell ref="M82:N82"/>
-    <mergeCell ref="M83:N83"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="M79:N79"/>
-    <mergeCell ref="M80:N80"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M71:N71"/>
-    <mergeCell ref="M72:N72"/>
-    <mergeCell ref="M73:N73"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M76:N76"/>
-    <mergeCell ref="M77:N77"/>
-    <mergeCell ref="M78:N78"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="J40:O40"/>
-    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="J55:N57"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="J74:K74"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="J78:K78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="J97:K97"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="J91:K91"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="M69:N69"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="J95:K95"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="A81:D81"/>
   </mergeCells>
   <conditionalFormatting sqref="E69">
     <cfRule type="duplicateValues" dxfId="170" priority="209"/>

</xml_diff>